<commit_message>
Updates in ELN Setup
</commit_message>
<xml_diff>
--- a/Abbaspour/ELNs/Ergänzendes Laborbuch_Kinetik_1.xlsx
+++ b/Abbaspour/ELNs/Ergänzendes Laborbuch_Kinetik_1.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smaxbehr\Documents\GitHub\NFDI\Abschlussarbeiten_Behr\Abbaspour\ELNs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Abschlussarbeiten_Behr\Abbaspour\ELNs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F66369-762D-4D4E-B109-D5E60AEDD49F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Substances and Paramteres" sheetId="1" r:id="rId1"/>
+    <sheet name="Substances and Parameters" sheetId="1" r:id="rId1"/>
     <sheet name="Properties for JSON-file" sheetId="2" r:id="rId2"/>
     <sheet name="Additional Info (Units)" sheetId="3" r:id="rId3"/>
     <sheet name="Reactorspecification" sheetId="4" r:id="rId4"/>
@@ -23,17 +24,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -248,9 +238,6 @@
     <t>C18H18N4O6S4</t>
   </si>
   <si>
-    <t>hasStoichiometriCoefficient</t>
-  </si>
-  <si>
     <t>hasDirect_OrderCoefficient</t>
   </si>
   <si>
@@ -432,12 +419,15 @@
   </si>
   <si>
     <t>Additional ELN Page 2: Properties for JSON-file</t>
+  </si>
+  <si>
+    <t>hasStoichiometricCoefficient</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -781,7 +771,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1092,28 +1082,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
@@ -1121,9 +1111,9 @@
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -1141,9 +1131,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>0</v>
@@ -1161,9 +1151,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>69</v>
+        <v>130</v>
       </c>
       <c r="B5" s="2">
         <v>0</v>
@@ -1181,9 +1171,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B6" s="2">
         <v>0</v>
@@ -1201,9 +1191,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B7" s="2">
         <v>0</v>
@@ -1221,27 +1211,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="F8" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>13</v>
       </c>
@@ -1261,9 +1251,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B10" s="3">
         <v>9.6666666666666705E-10</v>
@@ -1281,29 +1271,29 @@
         <v>4.6243132629629627E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>83</v>
-      </c>
       <c r="C11" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B12" s="3">
         <v>8.3333333333333299E-8</v>
@@ -1321,29 +1311,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>112</v>
-      </c>
       <c r="C13" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="36" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B14" s="37"/>
       <c r="C14" s="18"/>
@@ -1351,9 +1341,9 @@
       <c r="E14" s="18"/>
       <c r="F14" s="18"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B15" s="2">
         <v>0.93600000000000005</v>
@@ -1363,12 +1353,12 @@
       <c r="E15" s="18"/>
       <c r="F15" s="18"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C16" s="18"/>
       <c r="D16" s="18"/>
@@ -1376,9 +1366,9 @@
       <c r="F16" s="18"/>
       <c r="H16" s="21"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B17" s="20">
         <v>1.2</v>
@@ -1388,29 +1378,29 @@
       <c r="E17" s="18"/>
       <c r="F17" s="18"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>121</v>
       </c>
       <c r="C18" s="18"/>
       <c r="D18" s="18"/>
       <c r="E18" s="18"/>
       <c r="F18" s="18"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>15</v>
@@ -1425,13 +1415,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>'Dropdown Options'!$A$2:$A$3</xm:f>
           </x14:formula1>
           <xm:sqref>B9:F9 B19 B20</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000001000000}">
           <x14:formula1>
             <xm:f>'Dropdown Options'!$B$2:$B$5</xm:f>
           </x14:formula1>
@@ -1444,48 +1434,48 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.5546875" style="10" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.5546875" style="10"/>
+    <col min="1" max="1" width="45.5703125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="11.5703125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
         <v>37</v>
       </c>
       <c r="G1" s="7"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
       <c r="F2" s="15"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C3" s="38"/>
       <c r="D3" s="38"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>0</v>
@@ -1497,7 +1487,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>10</v>
       </c>
@@ -1511,7 +1501,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>11</v>
       </c>
@@ -1525,7 +1515,7 @@
         <v>375.15</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>12</v>
       </c>
@@ -1539,7 +1529,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>17</v>
       </c>
@@ -1553,7 +1543,7 @@
         <v>513.61900000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>18</v>
       </c>
@@ -1567,7 +1557,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>20</v>
       </c>
@@ -1581,7 +1571,7 @@
         <v>-4356</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>21</v>
       </c>
@@ -1595,7 +1585,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="210" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>23</v>
       </c>
@@ -1603,13 +1593,13 @@
         <v>62</v>
       </c>
       <c r="C12" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>24</v>
       </c>
@@ -1623,7 +1613,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>27</v>
       </c>
@@ -1637,7 +1627,7 @@
         <v>647.14</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>17</v>
       </c>
@@ -1651,7 +1641,7 @@
         <v>513.61900000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>28</v>
       </c>
@@ -1665,7 +1655,7 @@
         <v>22064000</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>29</v>
       </c>
@@ -1679,7 +1669,7 @@
         <v>5.595E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>30</v>
       </c>
@@ -1693,7 +1683,7 @@
         <v>0.22900000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>31</v>
       </c>
@@ -1707,7 +1697,7 @@
         <v>0.34399999999999997</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>32</v>
       </c>
@@ -1721,7 +1711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>33</v>
       </c>
@@ -1735,7 +1725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>34</v>
       </c>
@@ -1749,7 +1739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>35</v>
       </c>
@@ -1763,7 +1753,7 @@
         <v>1.14199E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>36</v>
       </c>
@@ -1777,7 +1767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>44</v>
       </c>
@@ -1791,7 +1781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>45</v>
       </c>
@@ -1805,7 +1795,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>46</v>
       </c>
@@ -1819,7 +1809,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>47</v>
       </c>
@@ -1833,7 +1823,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>48</v>
       </c>
@@ -1847,7 +1837,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>49</v>
       </c>
@@ -1861,7 +1851,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>50</v>
       </c>
@@ -1875,7 +1865,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>51</v>
       </c>
@@ -1889,7 +1879,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>52</v>
       </c>
@@ -1913,38 +1903,38 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C3" s="38"/>
       <c r="D3" s="38"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>0</v>
@@ -1956,7 +1946,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>18</v>
       </c>
@@ -1970,12 +1960,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>65</v>
@@ -1984,12 +1974,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>65</v>
@@ -1998,7 +1988,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>25</v>
       </c>
@@ -2012,7 +2002,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>26</v>
       </c>
@@ -2026,7 +2016,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>38</v>
       </c>
@@ -2040,7 +2030,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>39</v>
       </c>
@@ -2054,7 +2044,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>40</v>
       </c>
@@ -2068,7 +2058,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>41</v>
       </c>
@@ -2082,7 +2072,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>42</v>
       </c>
@@ -2096,7 +2086,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>43</v>
       </c>
@@ -2110,7 +2100,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>43</v>
       </c>
@@ -2133,142 +2123,142 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B3" s="23">
         <v>101325</v>
       </c>
       <c r="G3" s="17"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>58</v>
       </c>
       <c r="G4" s="17"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B5" s="23">
         <v>120</v>
       </c>
       <c r="G5" s="17"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B7" s="23">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B9" s="6">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="B11" s="4">
         <v>1.6000000000000001E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B14" s="6">
         <v>7.9999999999999996E-6</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B16" s="4">
         <v>1</v>
@@ -2280,13 +2270,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000000000000}">
           <x14:formula1>
             <xm:f>'Dropdown Options'!$C$1:$C$4</xm:f>
           </x14:formula1>
           <xm:sqref>B13</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000001000000}">
           <x14:formula1>
             <xm:f>'Dropdown Options'!$D$1:$D$4</xm:f>
           </x14:formula1>
@@ -2299,90 +2289,90 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5546875" customWidth="1"/>
-    <col min="5" max="5" width="28.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="28.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C1" s="31" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D1" s="24">
         <v>0</v>
       </c>
       <c r="E1" s="25" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D2" s="26">
         <v>1</v>
       </c>
       <c r="E2" s="27" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D3" s="26">
         <v>2</v>
       </c>
       <c r="E3" s="28" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="32"/>
       <c r="B4" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D4" s="26">
         <v>3</v>
       </c>
       <c r="E4" s="28" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="33"/>
       <c r="B5" s="33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C5" s="33"/>
       <c r="D5" s="29"/>

</xml_diff>